<commit_message>
just for recording: just parse phases are implemented.
</commit_message>
<xml_diff>
--- a/meta/telegrams/ApiDeleteTelegram.xlsx
+++ b/meta/telegrams/ApiDeleteTelegram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/objects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/cacco/oplux/oplux-meta/meta/telegrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D37B1A5-BB85-D74D-8E25-E356DFA8DC21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E95401-F2B6-B147-8CD2-494F4AC9CA8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="1440" windowWidth="24320" windowHeight="14120" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13680" yWindow="7080" windowWidth="24320" windowHeight="14120" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,16 @@
   <definedNames>
     <definedName name="accessScope">config!$B$4:$B$6</definedName>
     <definedName name="accessScope2">config!$B$4:$B$5</definedName>
-    <definedName name="adjustDefaultValue">config!$J$4:$J$5</definedName>
-    <definedName name="adjustFiledName">config!$H$4:$H$5</definedName>
-    <definedName name="createToString">config!$F$4:$F$5</definedName>
-    <definedName name="isAbstract">config!$D$4:$D$5</definedName>
+    <definedName name="adjustDefaultValue">config!$N$4:$N$5</definedName>
+    <definedName name="adjustFiledName">config!$L$4:$L$5</definedName>
+    <definedName name="createToString">config!$J$4:$J$5</definedName>
+    <definedName name="isAbstract">config!$H$4:$H$5</definedName>
+    <definedName name="isData">config!$F$4:$F$5</definedName>
+    <definedName name="isFinal">config!$D$4:$D$5</definedName>
     <definedName name="Submit有無" localSheetId="1">#REF!</definedName>
     <definedName name="Submit有無">#REF!</definedName>
-    <definedName name="toString">config!$F$4:$F$5</definedName>
+    <definedName name="theOther">config!$P$4:$P$5</definedName>
+    <definedName name="toString">config!$J$4:$J$5</definedName>
     <definedName name="Validate実装パターン" localSheetId="1">#REF!</definedName>
     <definedName name="Validate実装パターン">#REF!</definedName>
     <definedName name="チェック種別" localSheetId="1">#REF!</definedName>
@@ -54,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>クラス名</t>
   </si>
@@ -290,6 +293,56 @@
   <si>
     <t>アノテーション</t>
     <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>dataクラス</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* kotlin 独自 */</t>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">ドクジ </t>
+    </rPh>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>抽象クラス</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">チュウショウクラス </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ファイナル</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>○</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>その他</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>総称型</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">ソウショウガタ </t>
+    </rPh>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>※ クラスのGenericを定義するために使用します。</t>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">テイギスル </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">シヨウシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>public</t>
   </si>
 </sst>
 </file>
@@ -401,7 +454,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -894,6 +947,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1036,32 +1115,36 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -1475,10 +1558,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1529,7 +1612,7 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="75"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
@@ -1541,7 +1624,7 @@
       </c>
       <c r="D7" s="40"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="75"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
@@ -1553,111 +1636,115 @@
       </c>
       <c r="D8" s="40"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="75"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:12" s="35" customFormat="1">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="75"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="35" customFormat="1">
+      <c r="A10" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="78" t="s">
+      <c r="B10" s="77"/>
+      <c r="C10" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="79"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="83" t="s">
+      <c r="D10" s="72"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="83"/>
-    </row>
-    <row r="10" spans="1:12" s="35" customFormat="1">
-      <c r="A10" s="81" t="s">
+    </row>
+    <row r="11" spans="1:12" s="35" customFormat="1">
+      <c r="A11" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="73"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-    </row>
-    <row r="13" spans="1:12" s="35" customFormat="1">
-      <c r="A13" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="52"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:12" s="35" customFormat="1">
       <c r="A14" s="50" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B14" s="51"/>
       <c r="C14" s="52" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
     </row>
     <row r="15" spans="1:12" s="35" customFormat="1">
       <c r="A15" s="50" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B15" s="51"/>
-      <c r="C15" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15"/>
+      <c r="C15" s="52"/>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
     </row>
     <row r="16" spans="1:12" s="35" customFormat="1">
-      <c r="A16" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="70"/>
-      <c r="C16" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>41</v>
-      </c>
+      <c r="A16" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="51"/>
+      <c r="C16" s="52"/>
+      <c r="D16"/>
+      <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>
@@ -1666,70 +1753,77 @@
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="39"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="39"/>
-    </row>
-    <row r="22" spans="1:10">
+    <row r="17" spans="1:12" s="35" customFormat="1">
+      <c r="A17" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="51"/>
+      <c r="C17" s="52"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="1:12" s="35" customFormat="1">
+      <c r="A18" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="51"/>
+      <c r="C18" s="52"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:12" s="35" customFormat="1">
+      <c r="A19" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="51"/>
+      <c r="C19" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:12" s="35" customFormat="1">
+      <c r="A20" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="51"/>
+      <c r="C20" s="52"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:12" s="35" customFormat="1">
+      <c r="A21" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="70"/>
+      <c r="C21" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -1738,186 +1832,189 @@
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
     </row>
-    <row r="23" spans="1:10" s="35" customFormat="1">
+    <row r="23" spans="1:12">
       <c r="A23" s="32" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="53"/>
-    </row>
-    <row r="24" spans="1:10" s="35" customFormat="1">
-      <c r="A24" s="54" t="s">
+      <c r="F23" s="34"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="37"/>
+      <c r="C24" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="39"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="39"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:12" s="35" customFormat="1">
+      <c r="A28" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="53"/>
+    </row>
+    <row r="29" spans="1:12" s="35" customFormat="1">
+      <c r="A29" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B29" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="56"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
-    </row>
-    <row r="25" spans="1:10" s="35" customFormat="1">
-      <c r="A25" s="58"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="62"/>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25"/>
-    </row>
-    <row r="26" spans="1:10" s="35" customFormat="1">
-      <c r="A26" s="58"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="62"/>
-      <c r="H26"/>
-      <c r="I26"/>
-      <c r="J26"/>
-    </row>
-    <row r="27" spans="1:10" s="35" customFormat="1">
-      <c r="A27" s="65"/>
-      <c r="B27" s="66"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="62"/>
-      <c r="H27"/>
-      <c r="I27"/>
-      <c r="J27"/>
-    </row>
-    <row r="28" spans="1:10" s="35" customFormat="1">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="3" t="s">
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="56"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+    </row>
+    <row r="30" spans="1:12" s="35" customFormat="1">
+      <c r="A30" s="58"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="62"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:12" s="35" customFormat="1">
+      <c r="A31" s="58"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="62"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:12" s="35" customFormat="1">
+      <c r="A32" s="65"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="62"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="1:10" s="35" customFormat="1">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="15"/>
-    </row>
-    <row r="30" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A30" s="72" t="s">
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="15"/>
+    </row>
+    <row r="35" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A35" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="72" t="s">
+      <c r="B35" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="71" t="s">
+      <c r="C35" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="73" t="s">
+      <c r="D35" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="71" t="s">
+      <c r="E35" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="71" t="s">
+      <c r="F35" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="G30" s="71"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="9"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="72"/>
-      <c r="B31" s="72"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="71"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="15"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="19"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="15"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="15"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="19"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="15"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="19"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="15"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="9"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="19"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="23"/>
+      <c r="A36" s="79"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="30"/>
       <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10">
@@ -1929,7 +2026,7 @@
       <c r="F37" s="21"/>
       <c r="G37" s="22"/>
       <c r="H37" s="22"/>
-      <c r="I37" s="23"/>
+      <c r="I37" s="29"/>
       <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10">
@@ -1937,7 +2034,7 @@
       <c r="B38" s="20"/>
       <c r="C38" s="21"/>
       <c r="D38" s="21"/>
-      <c r="E38" s="31"/>
+      <c r="E38" s="21"/>
       <c r="F38" s="21"/>
       <c r="G38" s="22"/>
       <c r="H38" s="22"/>
@@ -1961,7 +2058,7 @@
       <c r="B40" s="20"/>
       <c r="C40" s="21"/>
       <c r="D40" s="21"/>
-      <c r="E40" s="31"/>
+      <c r="E40" s="21"/>
       <c r="F40" s="21"/>
       <c r="G40" s="22"/>
       <c r="H40" s="22"/>
@@ -1973,7 +2070,7 @@
       <c r="B41" s="20"/>
       <c r="C41" s="21"/>
       <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
+      <c r="E41" s="31"/>
       <c r="F41" s="21"/>
       <c r="G41" s="22"/>
       <c r="H41" s="22"/>
@@ -1997,7 +2094,7 @@
       <c r="B43" s="20"/>
       <c r="C43" s="21"/>
       <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
+      <c r="E43" s="31"/>
       <c r="F43" s="21"/>
       <c r="G43" s="22"/>
       <c r="H43" s="22"/>
@@ -2021,7 +2118,7 @@
       <c r="B45" s="20"/>
       <c r="C45" s="21"/>
       <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
+      <c r="E45" s="31"/>
       <c r="F45" s="21"/>
       <c r="G45" s="22"/>
       <c r="H45" s="22"/>
@@ -2029,38 +2126,110 @@
       <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="24"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="28"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="23"/>
       <c r="J46" s="15"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="19"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="15"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="19"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="15"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="19"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="15"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="19"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="15"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="24"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F30:G31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="F35:G36"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="D35:D36"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E62" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E67" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{D91A6F7B-4D29-2449-B2A6-B2DE56883681}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{D91A6F7B-4D29-2449-B2A6-B2DE56883681}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:C16" xr:uid="{B0E32580-3EF3-AE41-8E80-2DD2D7B8B160}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C21" xr:uid="{B0E32580-3EF3-AE41-8E80-2DD2D7B8B160}">
       <formula1>adjustDefaultValue</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{33BFBDB0-051A-4D45-80E7-0CED6C43D8C8}">
+      <formula1>isData</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{3AF994A6-7684-4F4B-8E47-3B581417E25B}">
+      <formula1>isFinal</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{61691BC2-585F-104A-9070-C3A4EAE37259}">
+      <formula1>isAbstract</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{7EBA0B23-7A38-354E-988E-F8CD334BB03D}">
+      <formula1>accessScope2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.59027777777777779" right="0.59027777777777779" top="0.59027777777777779" bottom="0.59027777777777779" header="0.51180555555555562" footer="0.11805555555555557"/>
@@ -2076,10 +2245,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -2087,16 +2256,20 @@
     <col min="1" max="3" width="8.83203125" style="43" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" style="43" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" style="43" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="43" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" style="43" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="43" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" style="43" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="43" bestFit="1" customWidth="1"/>
-    <col min="11" max="256" width="8.83203125" style="43" customWidth="1"/>
-    <col min="257" max="16384" width="10.83203125" style="43"/>
+    <col min="10" max="10" width="18.5" style="43" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="43" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="43" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="15" max="261" width="8.83203125" style="43" customWidth="1"/>
+    <col min="262" max="16384" width="10.83203125" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19">
+    <row r="1" spans="1:18" ht="19">
       <c r="A1" s="41" t="s">
         <v>21</v>
       </c>
@@ -2108,53 +2281,78 @@
       <c r="G1" s="41"/>
       <c r="H1" s="41"/>
       <c r="I1" s="41"/>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="42"/>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="R1" s="42"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="B3" s="44" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="J3" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="L3" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="N3" s="44" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="P3" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="B4" s="45"/>
-      <c r="D4" s="46"/>
-      <c r="F4" s="46"/>
+      <c r="D4" s="83" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>50</v>
+      </c>
       <c r="H4" s="46"/>
       <c r="J4" s="46"/>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="L4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="P4" s="46"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="B5" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="48" t="s">
-        <v>29</v>
-      </c>
+      <c r="D5" s="82"/>
+      <c r="F5" s="48"/>
       <c r="H5" s="48" t="s">
         <v>29</v>
       </c>
       <c r="J5" s="48" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="L5" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="48" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="B6" s="49"/>
     </row>
   </sheetData>

</xml_diff>